<commit_message>
linearregression.py | substituted first line by the dataset import
Main changes:
1. linearregression.py : imported dataset in order to avoid repeated
code;
2. xlsx file : changed name to correspond to the one in
datamanagement.py (swiss_travels)
</commit_message>
<xml_diff>
--- a/Data/RV6_swiss_travels.xlsx
+++ b/Data/RV6_swiss_travels.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Matias\Trabalho\Nova SBE\2016-2017\St. Gallen\Software Engineering for Economists\softwareengineering\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="0" windowWidth="25120" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="420" yWindow="0" windowWidth="25125" windowHeight="16125" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -24,13 +29,13 @@
     <t>year</t>
   </si>
   <si>
-    <t>Swiss travels</t>
+    <t>swiss_travels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###\ ###\ ###"/>
   </numFmts>
@@ -95,10 +100,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -427,15 +440,15 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -464,7 +477,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -493,7 +506,7 @@
         <v>6544.53935</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18">
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>

</xml_diff>